<commit_message>
Add image field in excel upload
</commit_message>
<xml_diff>
--- a/public/templates/Book-Import-Template.xlsx
+++ b/public/templates/Book-Import-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bookhub\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B715256F-A80F-4879-A70D-6FDA53FE0E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3A8832-E828-43C9-AF94-9A3952C148AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9DD50B20-475A-4F9F-9449-86A427C58EF4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Book Condition</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D018F96-49E5-43E9-A10D-55C1779A262D}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,9 +485,10 @@
     <col min="9" max="9" width="43.28515625" customWidth="1"/>
     <col min="10" max="10" width="18.140625" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,6 +521,9 @@
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>